<commit_message>
Updated 'Product Backlog' user stories
- Added column for noting which stories should be completed by the halfway point
- Changed risk evaluating system
- Changed risk assessment of some stories

- Todo: Finalize size and risk assessment of each stories
- Todo: Transfer final assessments to a new GitHub project page
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\OneDrive\Desktop\Github\Personal-Projects\Python\Python Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\OneDrive\Desktop\Github\APPvengers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E11CBA-82F5-4CAF-8EF2-351FDAA88D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196C1348-7088-4F7E-8012-25167BD4D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t>Player</t>
   </si>
@@ -197,13 +197,20 @@
   </si>
   <si>
     <t>Size (1-5)</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>Implement for
+halfway point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,8 +267,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +330,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -397,7 +416,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -408,8 +427,9 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -450,13 +470,26 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
     <cellStyle name="20% - Accent6" xfId="9" builtinId="50"/>
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="8" builtinId="39"/>
+    <cellStyle name="Accent2" xfId="10" builtinId="33"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="4" builtinId="20"/>
@@ -761,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
@@ -772,30 +805,37 @@
     <col min="1" max="1" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="155.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.7265625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="17.6328125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C1" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E1" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H2" s="17">
+        <v>13</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -805,17 +845,21 @@
       <c r="C3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="12">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="13">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H3" s="9">
+        <v>8</v>
+      </c>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -825,17 +869,20 @@
       <c r="C4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="12">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H4" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -845,14 +892,17 @@
       <c r="C5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="12">
-        <v>2</v>
-      </c>
-      <c r="G5" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -862,14 +912,17 @@
       <c r="C6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="11">
-        <v>3</v>
-      </c>
-      <c r="G6" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D6" s="12">
+        <v>2</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -879,11 +932,17 @@
       <c r="C7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D7" s="12">
+        <v>2</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
@@ -893,11 +952,14 @@
       <c r="C8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8" s="12">
+        <v>2</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -908,16 +970,17 @@
         <v>57</v>
       </c>
       <c r="D9" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -930,8 +993,9 @@
       <c r="D12" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -944,8 +1008,11 @@
       <c r="D13" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E13" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
@@ -958,8 +1025,9 @@
       <c r="D14" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
@@ -972,8 +1040,9 @@
       <c r="D15" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
@@ -986,8 +1055,11 @@
       <c r="D16" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E16" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
@@ -998,16 +1070,19 @@
         <v>56</v>
       </c>
       <c r="D17" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
@@ -1017,11 +1092,12 @@
       <c r="C20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D20" s="10">
+        <v>5</v>
+      </c>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
@@ -1031,17 +1107,18 @@
       <c r="C21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D21" s="10">
+        <v>5</v>
+      </c>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
@@ -1052,10 +1129,11 @@
         <v>57</v>
       </c>
       <c r="D24" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
         <v>36</v>
       </c>
@@ -1065,17 +1143,18 @@
       <c r="C25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D25" s="17">
+        <v>13</v>
+      </c>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="7" t="s">
         <v>39</v>
       </c>
@@ -1086,16 +1165,17 @@
         <v>57</v>
       </c>
       <c r="D28" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="30" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
         <v>42</v>
       </c>
@@ -1106,10 +1186,11 @@
         <v>57</v>
       </c>
       <c r="D31" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="7" t="s">
         <v>44</v>
       </c>
@@ -1120,16 +1201,17 @@
         <v>57</v>
       </c>
       <c r="D32" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="34" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="7" t="s">
         <v>47</v>
       </c>
@@ -1142,8 +1224,9 @@
       <c r="D35" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="7" t="s">
         <v>49</v>
       </c>
@@ -1156,14 +1239,15 @@
       <c r="D36" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="38" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="38" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="7" t="s">
         <v>52</v>
       </c>
@@ -1176,6 +1260,7 @@
       <c r="D39" s="12">
         <v>2</v>
       </c>
+      <c r="E39" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>